<commit_message>
1.0.8 - Hyppy ja osuma-äänet
</commit_message>
<xml_diff>
--- a/testausdokumentti.xlsx
+++ b/testausdokumentti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Projektit\EndlessRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6DC133-C7D2-4593-B0B0-5953B8E3DD16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98C19A3-1B6C-443A-9AEB-3D6D31B561F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3525" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>Ohjelmiston tuotantoversion testausdokumentti</t>
   </si>
@@ -145,6 +145,24 @@
   </si>
   <si>
     <t>Uusi pelaajahahmo on nyt lisätty peliin</t>
+  </si>
+  <si>
+    <t>Testi 5</t>
+  </si>
+  <si>
+    <t>1.0.8</t>
+  </si>
+  <si>
+    <t>Peliin lisättyjä ääniä</t>
+  </si>
+  <si>
+    <t>Hyppy ja osuma-äänet toistuvat oikeaan aikaan</t>
+  </si>
+  <si>
+    <t>Äänet lisättiin peliin onnistuneesti</t>
+  </si>
+  <si>
+    <t>Äänet toimivat moitteettomasti</t>
   </si>
 </sst>
 </file>
@@ -634,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +1017,92 @@
         <v>39</v>
       </c>
     </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="4"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="6">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1.0.9 - Boksi tekstuurit
</commit_message>
<xml_diff>
--- a/testausdokumentti.xlsx
+++ b/testausdokumentti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Projektit\EndlessRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98C19A3-1B6C-443A-9AEB-3D6D31B561F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B9FF3D-FD95-4FFB-BEE1-8016DC0CB81C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="2610" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
   <si>
     <t>Ohjelmiston tuotantoversion testausdokumentti</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t>Äänet toimivat moitteettomasti</t>
+  </si>
+  <si>
+    <t>Testi 6</t>
+  </si>
+  <si>
+    <t>1.0.9</t>
+  </si>
+  <si>
+    <t>Boksien tekstuureita ja niiden istuvuutta</t>
+  </si>
+  <si>
+    <t>Boksien tekstuurit toimivat normaalisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boksien tekstuurit toimivat  </t>
+  </si>
+  <si>
+    <t>Lisättiin bokseille uusi ulkonäkö onnistuneesti</t>
   </si>
 </sst>
 </file>
@@ -652,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,6 +1121,92 @@
         <v>44</v>
       </c>
     </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="4"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="6">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>